<commit_message>
Cập nhật SRS, changelog, file Excel, và khởi tạo thư mục design
</commit_message>
<xml_diff>
--- a/Documents/Template QLDA.xlsx
+++ b/Documents/Template QLDA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator.DESKTOP-98TGIBL\Documents\Zalo Received Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator.DESKTOP-98TGIBL\Desktop\Nhom-9-PTTKPM-N04\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC58C717-DC6B-432D-8A3B-37D3E8B8615D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5303DC0E-97F5-48A3-B5B9-9B02DB90938B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,8 +43,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -123,12 +145,6 @@
     <t>Jens Martensson</t>
   </si>
   <si>
-    <t>Nuria Acevedo</t>
-  </si>
-  <si>
-    <t>Olivia Wilson</t>
-  </si>
-  <si>
     <t>Project start:</t>
   </si>
   <si>
@@ -153,21 +169,9 @@
     <t>Planning</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>Tạo schedule</t>
   </si>
   <si>
-    <t>Xác định các vấn đề/chức năng trong TK</t>
-  </si>
-  <si>
-    <t>Wireframe và prototype</t>
-  </si>
-  <si>
-    <t>Hoàn thiện thiết kế</t>
-  </si>
-  <si>
     <t>Kiểm tra thiết kế</t>
   </si>
   <si>
@@ -241,6 +245,21 @@
   </si>
   <si>
     <t>Nguyễn Văn Luân</t>
+  </si>
+  <si>
+    <t>User interface sketch</t>
+  </si>
+  <si>
+    <t>Identify functions</t>
+  </si>
+  <si>
+    <t>Specification testing</t>
+  </si>
+  <si>
+    <t>Complete design</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Luân, Trần Đức Long</t>
   </si>
 </sst>
 </file>
@@ -1171,22 +1190,22 @@
     <xf numFmtId="164" fontId="19" fillId="10" borderId="5" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1198,17 +1217,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1808,17 +1827,17 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL45"/>
+  <dimension ref="A1:BL44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Z2"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="G27" sqref="A11:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.69921875" style="13" customWidth="1"/>
     <col min="2" max="2" width="51.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.69921875" customWidth="1"/>
+    <col min="3" max="3" width="29.296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.69921875" customWidth="1"/>
     <col min="5" max="5" width="10.69921875" style="2" customWidth="1"/>
     <col min="6" max="6" width="10.69921875" customWidth="1"/>
@@ -1829,8 +1848,8 @@
   <sheetData>
     <row r="1" spans="1:64" ht="90" customHeight="1" x14ac:dyDescent="1.05">
       <c r="A1" s="14"/>
-      <c r="B1" s="132" t="s">
-        <v>59</v>
+      <c r="B1" s="118" t="s">
+        <v>53</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="19"/>
@@ -1838,7 +1857,7 @@
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
       <c r="I1" s="127" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J1" s="128"/>
       <c r="K1" s="128"/>
@@ -1862,7 +1881,7 @@
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B2" s="96" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C2" s="97" t="s">
         <v>20</v>
@@ -1871,7 +1890,7 @@
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
       <c r="I2" s="127" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J2" s="128"/>
       <c r="K2" s="128"/>
@@ -1895,10 +1914,10 @@
     </row>
     <row r="3" spans="1:64" ht="25.2" x14ac:dyDescent="0.6">
       <c r="B3" s="96" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C3" s="97" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="23"/>
@@ -1925,7 +1944,7 @@
     <row r="4" spans="1:64" ht="25.2" x14ac:dyDescent="0.6">
       <c r="B4" s="96"/>
       <c r="C4" s="97" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="23"/>
@@ -1949,10 +1968,10 @@
       <c r="Y4" s="106"/>
       <c r="Z4" s="106"/>
     </row>
-    <row r="5" spans="1:64" ht="23.55" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:64" ht="25.2" x14ac:dyDescent="0.6">
       <c r="B5" s="96"/>
       <c r="C5" s="97" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23"/>
@@ -1976,11 +1995,11 @@
       <c r="Y5" s="106"/>
       <c r="Z5" s="106"/>
     </row>
-    <row r="6" spans="1:64" s="26" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:64" s="26" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="25"/>
       <c r="C6" s="108" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="28"/>
@@ -1989,105 +2008,105 @@
       <c r="A7" s="14"/>
       <c r="B7" s="29"/>
       <c r="C7" s="108" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E7" s="30"/>
-      <c r="I7" s="131">
+      <c r="I7" s="121">
         <f>I8</f>
         <v>45635</v>
       </c>
-      <c r="J7" s="129"/>
-      <c r="K7" s="129"/>
-      <c r="L7" s="129"/>
-      <c r="M7" s="129"/>
-      <c r="N7" s="129"/>
-      <c r="O7" s="129"/>
-      <c r="P7" s="129">
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
+      <c r="L7" s="119"/>
+      <c r="M7" s="119"/>
+      <c r="N7" s="119"/>
+      <c r="O7" s="119"/>
+      <c r="P7" s="119">
         <f>P8</f>
         <v>45642</v>
       </c>
-      <c r="Q7" s="129"/>
-      <c r="R7" s="129"/>
-      <c r="S7" s="129"/>
-      <c r="T7" s="129"/>
-      <c r="U7" s="129"/>
-      <c r="V7" s="129"/>
-      <c r="W7" s="129">
+      <c r="Q7" s="119"/>
+      <c r="R7" s="119"/>
+      <c r="S7" s="119"/>
+      <c r="T7" s="119"/>
+      <c r="U7" s="119"/>
+      <c r="V7" s="119"/>
+      <c r="W7" s="119">
         <f>W8</f>
         <v>45649</v>
       </c>
-      <c r="X7" s="129"/>
-      <c r="Y7" s="129"/>
-      <c r="Z7" s="129"/>
-      <c r="AA7" s="129"/>
-      <c r="AB7" s="129"/>
-      <c r="AC7" s="129"/>
-      <c r="AD7" s="129">
+      <c r="X7" s="119"/>
+      <c r="Y7" s="119"/>
+      <c r="Z7" s="119"/>
+      <c r="AA7" s="119"/>
+      <c r="AB7" s="119"/>
+      <c r="AC7" s="119"/>
+      <c r="AD7" s="119">
         <f>AD8</f>
         <v>45656</v>
       </c>
-      <c r="AE7" s="129"/>
-      <c r="AF7" s="129"/>
-      <c r="AG7" s="129"/>
-      <c r="AH7" s="129"/>
-      <c r="AI7" s="129"/>
-      <c r="AJ7" s="129"/>
-      <c r="AK7" s="129">
+      <c r="AE7" s="119"/>
+      <c r="AF7" s="119"/>
+      <c r="AG7" s="119"/>
+      <c r="AH7" s="119"/>
+      <c r="AI7" s="119"/>
+      <c r="AJ7" s="119"/>
+      <c r="AK7" s="119">
         <f>AK8</f>
         <v>45663</v>
       </c>
-      <c r="AL7" s="129"/>
-      <c r="AM7" s="129"/>
-      <c r="AN7" s="129"/>
-      <c r="AO7" s="129"/>
-      <c r="AP7" s="129"/>
-      <c r="AQ7" s="129"/>
-      <c r="AR7" s="129">
+      <c r="AL7" s="119"/>
+      <c r="AM7" s="119"/>
+      <c r="AN7" s="119"/>
+      <c r="AO7" s="119"/>
+      <c r="AP7" s="119"/>
+      <c r="AQ7" s="119"/>
+      <c r="AR7" s="119">
         <f>AR8</f>
         <v>45670</v>
       </c>
-      <c r="AS7" s="129"/>
-      <c r="AT7" s="129"/>
-      <c r="AU7" s="129"/>
-      <c r="AV7" s="129"/>
-      <c r="AW7" s="129"/>
-      <c r="AX7" s="129"/>
-      <c r="AY7" s="129">
+      <c r="AS7" s="119"/>
+      <c r="AT7" s="119"/>
+      <c r="AU7" s="119"/>
+      <c r="AV7" s="119"/>
+      <c r="AW7" s="119"/>
+      <c r="AX7" s="119"/>
+      <c r="AY7" s="119">
         <f>AY8</f>
         <v>45677</v>
       </c>
-      <c r="AZ7" s="129"/>
-      <c r="BA7" s="129"/>
-      <c r="BB7" s="129"/>
-      <c r="BC7" s="129"/>
-      <c r="BD7" s="129"/>
-      <c r="BE7" s="129"/>
-      <c r="BF7" s="129">
+      <c r="AZ7" s="119"/>
+      <c r="BA7" s="119"/>
+      <c r="BB7" s="119"/>
+      <c r="BC7" s="119"/>
+      <c r="BD7" s="119"/>
+      <c r="BE7" s="119"/>
+      <c r="BF7" s="119">
         <f>BF8</f>
         <v>45684</v>
       </c>
-      <c r="BG7" s="129"/>
-      <c r="BH7" s="129"/>
-      <c r="BI7" s="129"/>
-      <c r="BJ7" s="129"/>
-      <c r="BK7" s="129"/>
-      <c r="BL7" s="130"/>
+      <c r="BG7" s="119"/>
+      <c r="BH7" s="119"/>
+      <c r="BI7" s="119"/>
+      <c r="BJ7" s="119"/>
+      <c r="BK7" s="119"/>
+      <c r="BL7" s="120"/>
     </row>
     <row r="8" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="118"/>
-      <c r="B8" s="119" t="s">
+      <c r="A8" s="129"/>
+      <c r="B8" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="121" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="123" t="s">
+      <c r="C8" s="132" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="123" t="s">
+      <c r="E8" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="123" t="s">
+      <c r="F8" s="122" t="s">
         <v>4</v>
       </c>
       <c r="I8" s="31">
@@ -2316,12 +2335,12 @@
       </c>
     </row>
     <row r="9" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="118"/>
-      <c r="B9" s="120"/>
-      <c r="C9" s="122"/>
-      <c r="D9" s="122"/>
-      <c r="E9" s="122"/>
-      <c r="F9" s="122"/>
+      <c r="A9" s="129"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="123"/>
+      <c r="D9" s="123"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
       <c r="I9" s="34" t="str">
         <f t="shared" ref="I9:AN9" si="3">LEFT(TEXT(I8,"ddd"),1)</f>
         <v>M</v>
@@ -2618,9 +2637,12 @@
       <c r="BL10" s="39"/>
     </row>
     <row r="11" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
+      <c r="A11" s="14" cm="1">
+        <f t="array" aca="1" ref="A11" ca="1">A11:E35</f>
+        <v>0</v>
+      </c>
       <c r="B11" s="40" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" s="41"/>
       <c r="D11" s="42"/>
@@ -2628,7 +2650,7 @@
       <c r="F11" s="44"/>
       <c r="G11" s="17"/>
       <c r="H11" s="5" t="str">
-        <f t="shared" ref="H11:H42" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H11:H41" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I11" s="45"/>
@@ -2691,10 +2713,10 @@
     <row r="12" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="47" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D12" s="49">
         <v>1</v>
@@ -2772,13 +2794,13 @@
     <row r="13" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="52" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" s="53" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D13" s="54">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E13" s="55">
         <f>Project_Start</f>
@@ -2853,13 +2875,13 @@
     <row r="14" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="52" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C14" s="53" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D14" s="54">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E14" s="55">
         <f>Project_Start</f>
@@ -2934,13 +2956,13 @@
     <row r="15" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="52" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" s="53" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D15" s="54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="55">
         <f>F14</f>
@@ -3081,7 +3103,7 @@
     <row r="17" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="57" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C17" s="58"/>
       <c r="D17" s="59"/>
@@ -3096,26 +3118,26 @@
     <row r="18" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="62" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="C18" s="63" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="D18" s="64">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="E18" s="65">
-        <f>E16+1</f>
-        <v>1</v>
+        <f>E15+3</f>
+        <v>45644</v>
       </c>
       <c r="F18" s="65">
-        <f>E18+4</f>
-        <v>5</v>
+        <f>E18+1</f>
+        <v>45645</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="5">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I18" s="51"/>
       <c r="J18" s="51"/>
@@ -3177,26 +3199,26 @@
     <row r="19" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="62" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C19" s="63" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="D19" s="64">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="E19" s="65">
-        <f>E18+2</f>
-        <v>3</v>
+        <f>F18</f>
+        <v>45645</v>
       </c>
       <c r="F19" s="65">
-        <f>E19+5</f>
-        <v>8</v>
+        <f>E19+2</f>
+        <v>45647</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="5">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I19" s="51"/>
       <c r="J19" s="51"/>
@@ -3258,24 +3280,26 @@
     <row r="20" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="62" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C20" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="64"/>
+        <v>54</v>
+      </c>
+      <c r="D20" s="64">
+        <v>0.8</v>
+      </c>
       <c r="E20" s="65">
         <f>F19</f>
-        <v>8</v>
+        <v>45647</v>
       </c>
       <c r="F20" s="65">
-        <f>E20+3</f>
-        <v>11</v>
+        <f>E20+2</f>
+        <v>45649</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="5">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I20" s="51"/>
       <c r="J20" s="51"/>
@@ -3337,19 +3361,21 @@
     <row r="21" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="62" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="C21" s="63" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="64"/>
+        <v>62</v>
+      </c>
+      <c r="D21" s="64">
+        <v>1</v>
+      </c>
       <c r="E21" s="65">
-        <f>E20</f>
-        <v>8</v>
+        <f>F20</f>
+        <v>45649</v>
       </c>
       <c r="F21" s="65">
         <f>E21+2</f>
-        <v>10</v>
+        <v>45651</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="5">
@@ -3414,122 +3440,124 @@
       <c r="BL21" s="51"/>
     </row>
     <row r="22" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
-      <c r="B22" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="64"/>
-      <c r="E22" s="65">
-        <f>E21</f>
-        <v>8</v>
-      </c>
-      <c r="F22" s="65">
-        <f>E22+3</f>
-        <v>11</v>
-      </c>
+      <c r="A22" s="14"/>
+      <c r="B22" s="109" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="110"/>
+      <c r="D22" s="111"/>
+      <c r="E22" s="112"/>
+      <c r="F22" s="113"/>
       <c r="G22" s="17"/>
-      <c r="H22" s="5">
+      <c r="H22" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="51"/>
-      <c r="N22" s="51"/>
-      <c r="O22" s="51"/>
-      <c r="P22" s="51"/>
-      <c r="Q22" s="51"/>
-      <c r="R22" s="51"/>
-      <c r="S22" s="51"/>
-      <c r="T22" s="51"/>
-      <c r="U22" s="51"/>
-      <c r="V22" s="51"/>
-      <c r="W22" s="51"/>
-      <c r="X22" s="51"/>
-      <c r="Y22" s="51"/>
-      <c r="Z22" s="51"/>
-      <c r="AA22" s="51"/>
-      <c r="AB22" s="51"/>
-      <c r="AC22" s="51"/>
-      <c r="AD22" s="51"/>
-      <c r="AE22" s="51"/>
-      <c r="AF22" s="51"/>
-      <c r="AG22" s="51"/>
-      <c r="AH22" s="51"/>
-      <c r="AI22" s="51"/>
-      <c r="AJ22" s="51"/>
-      <c r="AK22" s="51"/>
-      <c r="AL22" s="51"/>
-      <c r="AM22" s="51"/>
-      <c r="AN22" s="51"/>
-      <c r="AO22" s="51"/>
-      <c r="AP22" s="51"/>
-      <c r="AQ22" s="51"/>
-      <c r="AR22" s="51"/>
-      <c r="AS22" s="51"/>
-      <c r="AT22" s="51"/>
-      <c r="AU22" s="51"/>
-      <c r="AV22" s="51"/>
-      <c r="AW22" s="51"/>
-      <c r="AX22" s="51"/>
-      <c r="AY22" s="51"/>
-      <c r="AZ22" s="51"/>
-      <c r="BA22" s="51"/>
-      <c r="BB22" s="51"/>
-      <c r="BC22" s="51"/>
-      <c r="BD22" s="51"/>
-      <c r="BE22" s="51"/>
-      <c r="BF22" s="51"/>
-      <c r="BG22" s="51"/>
-      <c r="BH22" s="51"/>
-      <c r="BI22" s="51"/>
-      <c r="BJ22" s="51"/>
-      <c r="BK22" s="51"/>
-      <c r="BL22" s="51"/>
+        <v/>
+      </c>
     </row>
     <row r="23" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
-      <c r="B23" s="109" t="s">
+      <c r="B23" s="114" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="115" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="116">
+        <v>1</v>
+      </c>
+      <c r="E23" s="117">
+        <f>F21</f>
+        <v>45651</v>
+      </c>
+      <c r="F23" s="117">
+        <f>E23+1</f>
+        <v>45652</v>
+      </c>
+      <c r="G23" s="17"/>
+      <c r="H23" s="5">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="51"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="51"/>
+      <c r="S23" s="51"/>
+      <c r="T23" s="51"/>
+      <c r="U23" s="51"/>
+      <c r="V23" s="51"/>
+      <c r="W23" s="51"/>
+      <c r="X23" s="51"/>
+      <c r="Y23" s="51"/>
+      <c r="Z23" s="51"/>
+      <c r="AA23" s="51"/>
+      <c r="AB23" s="51"/>
+      <c r="AC23" s="51"/>
+      <c r="AD23" s="51"/>
+      <c r="AE23" s="51"/>
+      <c r="AF23" s="51"/>
+      <c r="AG23" s="51"/>
+      <c r="AH23" s="51"/>
+      <c r="AI23" s="51"/>
+      <c r="AJ23" s="51"/>
+      <c r="AK23" s="51"/>
+      <c r="AL23" s="51"/>
+      <c r="AM23" s="51"/>
+      <c r="AN23" s="51"/>
+      <c r="AO23" s="51"/>
+      <c r="AP23" s="51"/>
+      <c r="AQ23" s="51"/>
+      <c r="AR23" s="51"/>
+      <c r="AS23" s="51"/>
+      <c r="AT23" s="51"/>
+      <c r="AU23" s="51"/>
+      <c r="AV23" s="51"/>
+      <c r="AW23" s="51"/>
+      <c r="AX23" s="51"/>
+      <c r="AY23" s="51"/>
+      <c r="AZ23" s="51"/>
+      <c r="BA23" s="51"/>
+      <c r="BB23" s="51"/>
+      <c r="BC23" s="51"/>
+      <c r="BD23" s="51"/>
+      <c r="BE23" s="51"/>
+      <c r="BF23" s="51"/>
+      <c r="BG23" s="51"/>
+      <c r="BH23" s="51"/>
+      <c r="BI23" s="51"/>
+      <c r="BJ23" s="51"/>
+      <c r="BK23" s="51"/>
+      <c r="BL23" s="51"/>
+    </row>
+    <row r="24" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="13"/>
+      <c r="B24" s="114" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="115" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="110"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="112"/>
-      <c r="F23" s="113"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
-      <c r="B24" s="114" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="115" t="s">
-        <v>21</v>
-      </c>
       <c r="D24" s="116">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="E24" s="117">
-        <f>E15+1</f>
-        <v>45642</v>
+        <f>F23</f>
+        <v>45652</v>
       </c>
       <c r="F24" s="117">
-        <f>E24+4</f>
-        <v>45646</v>
+        <f>E24+1</f>
+        <v>45653</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="5">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I24" s="51"/>
       <c r="J24" s="51"/>
@@ -3543,8 +3571,8 @@
       <c r="R24" s="51"/>
       <c r="S24" s="51"/>
       <c r="T24" s="51"/>
-      <c r="U24" s="51"/>
-      <c r="V24" s="51"/>
+      <c r="U24" s="56"/>
+      <c r="V24" s="56"/>
       <c r="W24" s="51"/>
       <c r="X24" s="51"/>
       <c r="Y24" s="51"/>
@@ -3591,26 +3619,26 @@
     <row r="25" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="114" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C25" s="115" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="D25" s="116">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="E25" s="117">
-        <f>E24+2</f>
-        <v>45644</v>
+        <f>F24</f>
+        <v>45653</v>
       </c>
       <c r="F25" s="117">
-        <f>E25+5</f>
-        <v>45649</v>
+        <f>E25+2</f>
+        <v>45655</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="5">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I25" s="51"/>
       <c r="J25" s="51"/>
@@ -3624,8 +3652,8 @@
       <c r="R25" s="51"/>
       <c r="S25" s="51"/>
       <c r="T25" s="51"/>
-      <c r="U25" s="56"/>
-      <c r="V25" s="56"/>
+      <c r="U25" s="51"/>
+      <c r="V25" s="51"/>
       <c r="W25" s="51"/>
       <c r="X25" s="51"/>
       <c r="Y25" s="51"/>
@@ -3672,24 +3700,26 @@
     <row r="26" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="114" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C26" s="115" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="116"/>
+        <v>54</v>
+      </c>
+      <c r="D26" s="116">
+        <v>0.9</v>
+      </c>
       <c r="E26" s="117">
         <f>F25</f>
-        <v>45649</v>
+        <v>45655</v>
       </c>
       <c r="F26" s="117">
-        <f>E26+3</f>
-        <v>45652</v>
+        <f>E26+2</f>
+        <v>45657</v>
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="5">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I26" s="51"/>
       <c r="J26" s="51"/>
@@ -3707,7 +3737,7 @@
       <c r="V26" s="51"/>
       <c r="W26" s="51"/>
       <c r="X26" s="51"/>
-      <c r="Y26" s="51"/>
+      <c r="Y26" s="56"/>
       <c r="Z26" s="51"/>
       <c r="AA26" s="51"/>
       <c r="AB26" s="51"/>
@@ -3751,24 +3781,26 @@
     <row r="27" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="114" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C27" s="115" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="116"/>
+        <v>57</v>
+      </c>
+      <c r="D27" s="116">
+        <v>0.9</v>
+      </c>
       <c r="E27" s="117">
-        <f>E26</f>
-        <v>45649</v>
+        <f>F26</f>
+        <v>45657</v>
       </c>
       <c r="F27" s="117">
-        <f>E27+2</f>
-        <v>45651</v>
+        <f>E27+1</f>
+        <v>45658</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="5">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I27" s="51"/>
       <c r="J27" s="51"/>
@@ -3786,7 +3818,7 @@
       <c r="V27" s="51"/>
       <c r="W27" s="51"/>
       <c r="X27" s="51"/>
-      <c r="Y27" s="56"/>
+      <c r="Y27" s="51"/>
       <c r="Z27" s="51"/>
       <c r="AA27" s="51"/>
       <c r="AB27" s="51"/>
@@ -3829,177 +3861,179 @@
     </row>
     <row r="28" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
-      <c r="B28" s="114" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="115" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="116"/>
-      <c r="E28" s="117">
-        <f>E27</f>
-        <v>45649</v>
-      </c>
-      <c r="F28" s="117">
-        <f>E28+3</f>
-        <v>45652</v>
-      </c>
+      <c r="B28" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="67"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="70"/>
       <c r="G28" s="17"/>
-      <c r="H28" s="5">
+      <c r="H28" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="I28" s="51"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="51"/>
-      <c r="P28" s="51"/>
-      <c r="Q28" s="51"/>
-      <c r="R28" s="51"/>
-      <c r="S28" s="51"/>
-      <c r="T28" s="51"/>
-      <c r="U28" s="51"/>
-      <c r="V28" s="51"/>
-      <c r="W28" s="51"/>
-      <c r="X28" s="51"/>
-      <c r="Y28" s="51"/>
-      <c r="Z28" s="51"/>
-      <c r="AA28" s="51"/>
-      <c r="AB28" s="51"/>
-      <c r="AC28" s="51"/>
-      <c r="AD28" s="51"/>
-      <c r="AE28" s="51"/>
-      <c r="AF28" s="51"/>
-      <c r="AG28" s="51"/>
-      <c r="AH28" s="51"/>
-      <c r="AI28" s="51"/>
-      <c r="AJ28" s="51"/>
-      <c r="AK28" s="51"/>
-      <c r="AL28" s="51"/>
-      <c r="AM28" s="51"/>
-      <c r="AN28" s="51"/>
-      <c r="AO28" s="51"/>
-      <c r="AP28" s="51"/>
-      <c r="AQ28" s="51"/>
-      <c r="AR28" s="51"/>
-      <c r="AS28" s="51"/>
-      <c r="AT28" s="51"/>
-      <c r="AU28" s="51"/>
-      <c r="AV28" s="51"/>
-      <c r="AW28" s="51"/>
-      <c r="AX28" s="51"/>
-      <c r="AY28" s="51"/>
-      <c r="AZ28" s="51"/>
-      <c r="BA28" s="51"/>
-      <c r="BB28" s="51"/>
-      <c r="BC28" s="51"/>
-      <c r="BD28" s="51"/>
-      <c r="BE28" s="51"/>
-      <c r="BF28" s="51"/>
-      <c r="BG28" s="51"/>
-      <c r="BH28" s="51"/>
-      <c r="BI28" s="51"/>
-      <c r="BJ28" s="51"/>
-      <c r="BK28" s="51"/>
-      <c r="BL28" s="51"/>
+        <v/>
+      </c>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="71"/>
+      <c r="M28" s="71"/>
+      <c r="N28" s="71"/>
+      <c r="O28" s="71"/>
+      <c r="P28" s="71"/>
+      <c r="Q28" s="71"/>
+      <c r="R28" s="71"/>
+      <c r="S28" s="71"/>
+      <c r="T28" s="71"/>
+      <c r="U28" s="71"/>
+      <c r="V28" s="71"/>
+      <c r="W28" s="71"/>
+      <c r="X28" s="71"/>
+      <c r="Y28" s="71"/>
+      <c r="Z28" s="71"/>
+      <c r="AA28" s="71"/>
+      <c r="AB28" s="71"/>
+      <c r="AC28" s="71"/>
+      <c r="AD28" s="71"/>
+      <c r="AE28" s="71"/>
+      <c r="AF28" s="71"/>
+      <c r="AG28" s="71"/>
+      <c r="AH28" s="71"/>
+      <c r="AI28" s="71"/>
+      <c r="AJ28" s="71"/>
+      <c r="AK28" s="71"/>
+      <c r="AL28" s="71"/>
+      <c r="AM28" s="71"/>
+      <c r="AN28" s="71"/>
+      <c r="AO28" s="71"/>
+      <c r="AP28" s="71"/>
+      <c r="AQ28" s="71"/>
+      <c r="AR28" s="71"/>
+      <c r="AS28" s="71"/>
+      <c r="AT28" s="71"/>
+      <c r="AU28" s="71"/>
+      <c r="AV28" s="71"/>
+      <c r="AW28" s="71"/>
+      <c r="AX28" s="71"/>
+      <c r="AY28" s="71"/>
+      <c r="AZ28" s="71"/>
+      <c r="BA28" s="71"/>
+      <c r="BB28" s="71"/>
+      <c r="BC28" s="71"/>
+      <c r="BD28" s="71"/>
+      <c r="BE28" s="71"/>
+      <c r="BF28" s="71"/>
+      <c r="BG28" s="71"/>
+      <c r="BH28" s="71"/>
+      <c r="BI28" s="71"/>
+      <c r="BJ28" s="71"/>
+      <c r="BK28" s="71"/>
+      <c r="BL28" s="71"/>
     </row>
     <row r="29" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
-      <c r="B29" s="66" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="67"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="70"/>
+      <c r="B29" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="73" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="74">
+        <v>0.5</v>
+      </c>
+      <c r="E29" s="75">
+        <f>F27+2</f>
+        <v>45660</v>
+      </c>
+      <c r="F29" s="75">
+        <f>E29+1</f>
+        <v>45661</v>
+      </c>
       <c r="G29" s="17"/>
-      <c r="H29" s="5" t="str">
+      <c r="H29" s="5">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I29" s="71"/>
-      <c r="J29" s="71"/>
-      <c r="K29" s="71"/>
-      <c r="L29" s="71"/>
-      <c r="M29" s="71"/>
-      <c r="N29" s="71"/>
-      <c r="O29" s="71"/>
-      <c r="P29" s="71"/>
-      <c r="Q29" s="71"/>
-      <c r="R29" s="71"/>
-      <c r="S29" s="71"/>
-      <c r="T29" s="71"/>
-      <c r="U29" s="71"/>
-      <c r="V29" s="71"/>
-      <c r="W29" s="71"/>
-      <c r="X29" s="71"/>
-      <c r="Y29" s="71"/>
-      <c r="Z29" s="71"/>
-      <c r="AA29" s="71"/>
-      <c r="AB29" s="71"/>
-      <c r="AC29" s="71"/>
-      <c r="AD29" s="71"/>
-      <c r="AE29" s="71"/>
-      <c r="AF29" s="71"/>
-      <c r="AG29" s="71"/>
-      <c r="AH29" s="71"/>
-      <c r="AI29" s="71"/>
-      <c r="AJ29" s="71"/>
-      <c r="AK29" s="71"/>
-      <c r="AL29" s="71"/>
-      <c r="AM29" s="71"/>
-      <c r="AN29" s="71"/>
-      <c r="AO29" s="71"/>
-      <c r="AP29" s="71"/>
-      <c r="AQ29" s="71"/>
-      <c r="AR29" s="71"/>
-      <c r="AS29" s="71"/>
-      <c r="AT29" s="71"/>
-      <c r="AU29" s="71"/>
-      <c r="AV29" s="71"/>
-      <c r="AW29" s="71"/>
-      <c r="AX29" s="71"/>
-      <c r="AY29" s="71"/>
-      <c r="AZ29" s="71"/>
-      <c r="BA29" s="71"/>
-      <c r="BB29" s="71"/>
-      <c r="BC29" s="71"/>
-      <c r="BD29" s="71"/>
-      <c r="BE29" s="71"/>
-      <c r="BF29" s="71"/>
-      <c r="BG29" s="71"/>
-      <c r="BH29" s="71"/>
-      <c r="BI29" s="71"/>
-      <c r="BJ29" s="71"/>
-      <c r="BK29" s="71"/>
-      <c r="BL29" s="71"/>
+        <v>2</v>
+      </c>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="51"/>
+      <c r="L29" s="51"/>
+      <c r="M29" s="51"/>
+      <c r="N29" s="51"/>
+      <c r="O29" s="51"/>
+      <c r="P29" s="51"/>
+      <c r="Q29" s="51"/>
+      <c r="R29" s="51"/>
+      <c r="S29" s="51"/>
+      <c r="T29" s="51"/>
+      <c r="U29" s="51"/>
+      <c r="V29" s="51"/>
+      <c r="W29" s="51"/>
+      <c r="X29" s="51"/>
+      <c r="Y29" s="51"/>
+      <c r="Z29" s="51"/>
+      <c r="AA29" s="51"/>
+      <c r="AB29" s="51"/>
+      <c r="AC29" s="51"/>
+      <c r="AD29" s="51"/>
+      <c r="AE29" s="51"/>
+      <c r="AF29" s="51"/>
+      <c r="AG29" s="51"/>
+      <c r="AH29" s="51"/>
+      <c r="AI29" s="51"/>
+      <c r="AJ29" s="51"/>
+      <c r="AK29" s="51"/>
+      <c r="AL29" s="51"/>
+      <c r="AM29" s="51"/>
+      <c r="AN29" s="51"/>
+      <c r="AO29" s="51"/>
+      <c r="AP29" s="51"/>
+      <c r="AQ29" s="51"/>
+      <c r="AR29" s="51"/>
+      <c r="AS29" s="51"/>
+      <c r="AT29" s="51"/>
+      <c r="AU29" s="51"/>
+      <c r="AV29" s="51"/>
+      <c r="AW29" s="51"/>
+      <c r="AX29" s="51"/>
+      <c r="AY29" s="51"/>
+      <c r="AZ29" s="51"/>
+      <c r="BA29" s="51"/>
+      <c r="BB29" s="51"/>
+      <c r="BC29" s="51"/>
+      <c r="BD29" s="51"/>
+      <c r="BE29" s="51"/>
+      <c r="BF29" s="51"/>
+      <c r="BG29" s="51"/>
+      <c r="BH29" s="51"/>
+      <c r="BI29" s="51"/>
+      <c r="BJ29" s="51"/>
+      <c r="BK29" s="51"/>
+      <c r="BL29" s="51"/>
     </row>
     <row r="30" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="72" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C30" s="73" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="D30" s="74">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E30" s="75">
-        <f>E12+15</f>
-        <v>45654</v>
+        <f>F29</f>
+        <v>45661</v>
       </c>
       <c r="F30" s="75">
-        <f>E30+5</f>
-        <v>45659</v>
+        <f>E30+4</f>
+        <v>45665</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="5">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I30" s="51"/>
       <c r="J30" s="51"/>
@@ -4061,21 +4095,21 @@
     <row r="31" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="72" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C31" s="73" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="D31" s="74">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="E31" s="75">
-        <f>F30+1</f>
-        <v>45660</v>
+        <f>F30</f>
+        <v>45665</v>
       </c>
       <c r="F31" s="75">
         <f>E31+4</f>
-        <v>45664</v>
+        <v>45669</v>
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="5">
@@ -4142,26 +4176,26 @@
     <row r="32" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="72" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C32" s="73" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="D32" s="74">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="E32" s="75">
-        <f>E31+5</f>
-        <v>45665</v>
+        <f>F31+1</f>
+        <v>45670</v>
       </c>
       <c r="F32" s="75">
-        <f>E32+5</f>
-        <v>45670</v>
+        <f>E32+4</f>
+        <v>45674</v>
       </c>
       <c r="G32" s="17"/>
       <c r="H32" s="5">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I32" s="51"/>
       <c r="J32" s="51"/>
@@ -4223,21 +4257,21 @@
     <row r="33" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="72" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C33" s="73" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="D33" s="74">
         <v>0.25</v>
       </c>
       <c r="E33" s="75">
-        <f>F32+1</f>
-        <v>45671</v>
+        <f>E31</f>
+        <v>45665</v>
       </c>
       <c r="F33" s="75">
         <f>E33+4</f>
-        <v>45675</v>
+        <v>45669</v>
       </c>
       <c r="G33" s="17"/>
       <c r="H33" s="5">
@@ -4303,179 +4337,179 @@
     </row>
     <row r="34" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13"/>
-      <c r="B34" s="72" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="74">
-        <v>0.25</v>
-      </c>
-      <c r="E34" s="75">
-        <f>E32</f>
-        <v>45665</v>
-      </c>
-      <c r="F34" s="75">
-        <f>E34+4</f>
-        <v>45669</v>
-      </c>
+      <c r="B34" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="77"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="80"/>
       <c r="G34" s="17"/>
-      <c r="H34" s="5">
+      <c r="H34" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="I34" s="51"/>
-      <c r="J34" s="51"/>
-      <c r="K34" s="51"/>
-      <c r="L34" s="51"/>
-      <c r="M34" s="51"/>
-      <c r="N34" s="51"/>
-      <c r="O34" s="51"/>
-      <c r="P34" s="51"/>
-      <c r="Q34" s="51"/>
-      <c r="R34" s="51"/>
-      <c r="S34" s="51"/>
-      <c r="T34" s="51"/>
-      <c r="U34" s="51"/>
-      <c r="V34" s="51"/>
-      <c r="W34" s="51"/>
-      <c r="X34" s="51"/>
-      <c r="Y34" s="51"/>
-      <c r="Z34" s="51"/>
-      <c r="AA34" s="51"/>
-      <c r="AB34" s="51"/>
-      <c r="AC34" s="51"/>
-      <c r="AD34" s="51"/>
-      <c r="AE34" s="51"/>
-      <c r="AF34" s="51"/>
-      <c r="AG34" s="51"/>
-      <c r="AH34" s="51"/>
-      <c r="AI34" s="51"/>
-      <c r="AJ34" s="51"/>
-      <c r="AK34" s="51"/>
-      <c r="AL34" s="51"/>
-      <c r="AM34" s="51"/>
-      <c r="AN34" s="51"/>
-      <c r="AO34" s="51"/>
-      <c r="AP34" s="51"/>
-      <c r="AQ34" s="51"/>
-      <c r="AR34" s="51"/>
-      <c r="AS34" s="51"/>
-      <c r="AT34" s="51"/>
-      <c r="AU34" s="51"/>
-      <c r="AV34" s="51"/>
-      <c r="AW34" s="51"/>
-      <c r="AX34" s="51"/>
-      <c r="AY34" s="51"/>
-      <c r="AZ34" s="51"/>
-      <c r="BA34" s="51"/>
-      <c r="BB34" s="51"/>
-      <c r="BC34" s="51"/>
-      <c r="BD34" s="51"/>
-      <c r="BE34" s="51"/>
-      <c r="BF34" s="51"/>
-      <c r="BG34" s="51"/>
-      <c r="BH34" s="51"/>
-      <c r="BI34" s="51"/>
-      <c r="BJ34" s="51"/>
-      <c r="BK34" s="51"/>
-      <c r="BL34" s="51"/>
+        <v/>
+      </c>
+      <c r="I34" s="81"/>
+      <c r="J34" s="81"/>
+      <c r="K34" s="81"/>
+      <c r="L34" s="81"/>
+      <c r="M34" s="81"/>
+      <c r="N34" s="81"/>
+      <c r="O34" s="81"/>
+      <c r="P34" s="81"/>
+      <c r="Q34" s="81"/>
+      <c r="R34" s="81"/>
+      <c r="S34" s="81"/>
+      <c r="T34" s="81"/>
+      <c r="U34" s="81"/>
+      <c r="V34" s="81"/>
+      <c r="W34" s="81"/>
+      <c r="X34" s="81"/>
+      <c r="Y34" s="81"/>
+      <c r="Z34" s="81"/>
+      <c r="AA34" s="81"/>
+      <c r="AB34" s="81"/>
+      <c r="AC34" s="81"/>
+      <c r="AD34" s="81"/>
+      <c r="AE34" s="81"/>
+      <c r="AF34" s="81"/>
+      <c r="AG34" s="81"/>
+      <c r="AH34" s="81"/>
+      <c r="AI34" s="81"/>
+      <c r="AJ34" s="81"/>
+      <c r="AK34" s="81"/>
+      <c r="AL34" s="81"/>
+      <c r="AM34" s="81"/>
+      <c r="AN34" s="81"/>
+      <c r="AO34" s="81"/>
+      <c r="AP34" s="81"/>
+      <c r="AQ34" s="81"/>
+      <c r="AR34" s="81"/>
+      <c r="AS34" s="81"/>
+      <c r="AT34" s="81"/>
+      <c r="AU34" s="81"/>
+      <c r="AV34" s="81"/>
+      <c r="AW34" s="81"/>
+      <c r="AX34" s="81"/>
+      <c r="AY34" s="81"/>
+      <c r="AZ34" s="81"/>
+      <c r="BA34" s="81"/>
+      <c r="BB34" s="81"/>
+      <c r="BC34" s="81"/>
+      <c r="BD34" s="81"/>
+      <c r="BE34" s="81"/>
+      <c r="BF34" s="81"/>
+      <c r="BG34" s="81"/>
+      <c r="BH34" s="81"/>
+      <c r="BI34" s="81"/>
+      <c r="BJ34" s="81"/>
+      <c r="BK34" s="81"/>
+      <c r="BL34" s="81"/>
     </row>
     <row r="35" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
-      <c r="B35" s="76" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="77"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="80"/>
+      <c r="B35" s="82" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="83" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="84">
+        <v>0.25</v>
+      </c>
+      <c r="E35" s="85">
+        <f>E29+2</f>
+        <v>45662</v>
+      </c>
+      <c r="F35" s="85">
+        <f>E35+3</f>
+        <v>45665</v>
+      </c>
       <c r="G35" s="17"/>
-      <c r="H35" s="5" t="str">
+      <c r="H35" s="5">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I35" s="81"/>
-      <c r="J35" s="81"/>
-      <c r="K35" s="81"/>
-      <c r="L35" s="81"/>
-      <c r="M35" s="81"/>
-      <c r="N35" s="81"/>
-      <c r="O35" s="81"/>
-      <c r="P35" s="81"/>
-      <c r="Q35" s="81"/>
-      <c r="R35" s="81"/>
-      <c r="S35" s="81"/>
-      <c r="T35" s="81"/>
-      <c r="U35" s="81"/>
-      <c r="V35" s="81"/>
-      <c r="W35" s="81"/>
-      <c r="X35" s="81"/>
-      <c r="Y35" s="81"/>
-      <c r="Z35" s="81"/>
-      <c r="AA35" s="81"/>
-      <c r="AB35" s="81"/>
-      <c r="AC35" s="81"/>
-      <c r="AD35" s="81"/>
-      <c r="AE35" s="81"/>
-      <c r="AF35" s="81"/>
-      <c r="AG35" s="81"/>
-      <c r="AH35" s="81"/>
-      <c r="AI35" s="81"/>
-      <c r="AJ35" s="81"/>
-      <c r="AK35" s="81"/>
-      <c r="AL35" s="81"/>
-      <c r="AM35" s="81"/>
-      <c r="AN35" s="81"/>
-      <c r="AO35" s="81"/>
-      <c r="AP35" s="81"/>
-      <c r="AQ35" s="81"/>
-      <c r="AR35" s="81"/>
-      <c r="AS35" s="81"/>
-      <c r="AT35" s="81"/>
-      <c r="AU35" s="81"/>
-      <c r="AV35" s="81"/>
-      <c r="AW35" s="81"/>
-      <c r="AX35" s="81"/>
-      <c r="AY35" s="81"/>
-      <c r="AZ35" s="81"/>
-      <c r="BA35" s="81"/>
-      <c r="BB35" s="81"/>
-      <c r="BC35" s="81"/>
-      <c r="BD35" s="81"/>
-      <c r="BE35" s="81"/>
-      <c r="BF35" s="81"/>
-      <c r="BG35" s="81"/>
-      <c r="BH35" s="81"/>
-      <c r="BI35" s="81"/>
-      <c r="BJ35" s="81"/>
-      <c r="BK35" s="81"/>
-      <c r="BL35" s="81"/>
+        <v>4</v>
+      </c>
+      <c r="I35" s="51"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="51"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="51"/>
+      <c r="N35" s="51"/>
+      <c r="O35" s="51"/>
+      <c r="P35" s="51"/>
+      <c r="Q35" s="51"/>
+      <c r="R35" s="51"/>
+      <c r="S35" s="51"/>
+      <c r="T35" s="51"/>
+      <c r="U35" s="51"/>
+      <c r="V35" s="51"/>
+      <c r="W35" s="51"/>
+      <c r="X35" s="51"/>
+      <c r="Y35" s="51"/>
+      <c r="Z35" s="51"/>
+      <c r="AA35" s="51"/>
+      <c r="AB35" s="51"/>
+      <c r="AC35" s="51"/>
+      <c r="AD35" s="51"/>
+      <c r="AE35" s="51"/>
+      <c r="AF35" s="51"/>
+      <c r="AG35" s="51"/>
+      <c r="AH35" s="51"/>
+      <c r="AI35" s="51"/>
+      <c r="AJ35" s="51"/>
+      <c r="AK35" s="51"/>
+      <c r="AL35" s="51"/>
+      <c r="AM35" s="51"/>
+      <c r="AN35" s="51"/>
+      <c r="AO35" s="51"/>
+      <c r="AP35" s="51"/>
+      <c r="AQ35" s="51"/>
+      <c r="AR35" s="51"/>
+      <c r="AS35" s="51"/>
+      <c r="AT35" s="51"/>
+      <c r="AU35" s="51"/>
+      <c r="AV35" s="51"/>
+      <c r="AW35" s="51"/>
+      <c r="AX35" s="51"/>
+      <c r="AY35" s="51"/>
+      <c r="AZ35" s="51"/>
+      <c r="BA35" s="51"/>
+      <c r="BB35" s="51"/>
+      <c r="BC35" s="51"/>
+      <c r="BD35" s="51"/>
+      <c r="BE35" s="51"/>
+      <c r="BF35" s="51"/>
+      <c r="BG35" s="51"/>
+      <c r="BH35" s="51"/>
+      <c r="BI35" s="51"/>
+      <c r="BJ35" s="51"/>
+      <c r="BK35" s="51"/>
+      <c r="BL35" s="51"/>
     </row>
     <row r="36" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="82" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C36" s="83" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D36" s="84">
         <v>0.25</v>
       </c>
       <c r="E36" s="85">
-        <f>E30+2</f>
-        <v>45656</v>
+        <f>F35</f>
+        <v>45665</v>
       </c>
       <c r="F36" s="85">
-        <f>E36+3</f>
-        <v>45659</v>
+        <f>E36+4</f>
+        <v>45669</v>
       </c>
       <c r="G36" s="17"/>
       <c r="H36" s="5">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I36" s="51"/>
       <c r="J36" s="51"/>
@@ -4537,26 +4571,26 @@
     <row r="37" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="82" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C37" s="83" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D37" s="84">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E37" s="85">
-        <f>F36</f>
-        <v>45659</v>
+        <f>F36+1</f>
+        <v>45670</v>
       </c>
       <c r="F37" s="85">
-        <f>E37+4</f>
-        <v>45663</v>
+        <f>E37+3</f>
+        <v>45673</v>
       </c>
       <c r="G37" s="17"/>
       <c r="H37" s="5">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I37" s="51"/>
       <c r="J37" s="51"/>
@@ -4617,28 +4651,13 @@
     </row>
     <row r="38" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
-      <c r="B38" s="82" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="83" t="s">
-        <v>23</v>
-      </c>
-      <c r="D38" s="84">
-        <v>0.5</v>
-      </c>
-      <c r="E38" s="85">
-        <f>F37+1</f>
-        <v>45664</v>
-      </c>
-      <c r="F38" s="85">
-        <f>E38+3</f>
-        <v>45667</v>
-      </c>
+      <c r="B38" s="82"/>
+      <c r="C38" s="83"/>
+      <c r="D38" s="84"/>
+      <c r="E38" s="85"/>
+      <c r="F38" s="85"/>
       <c r="G38" s="17"/>
-      <c r="H38" s="5">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
+      <c r="H38" s="5"/>
       <c r="I38" s="51"/>
       <c r="J38" s="51"/>
       <c r="K38" s="51"/>
@@ -4764,222 +4783,166 @@
     </row>
     <row r="40" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
-      <c r="B40" s="82"/>
-      <c r="C40" s="83"/>
-      <c r="D40" s="84"/>
-      <c r="E40" s="85"/>
-      <c r="F40" s="85"/>
+      <c r="B40" s="86"/>
+      <c r="C40" s="87"/>
+      <c r="D40" s="88"/>
+      <c r="E40" s="89"/>
+      <c r="F40" s="89"/>
       <c r="G40" s="17"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="51"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="51"/>
-      <c r="L40" s="51"/>
-      <c r="M40" s="51"/>
-      <c r="N40" s="51"/>
-      <c r="O40" s="51"/>
-      <c r="P40" s="51"/>
-      <c r="Q40" s="51"/>
-      <c r="R40" s="51"/>
-      <c r="S40" s="51"/>
-      <c r="T40" s="51"/>
-      <c r="U40" s="51"/>
-      <c r="V40" s="51"/>
-      <c r="W40" s="51"/>
-      <c r="X40" s="51"/>
-      <c r="Y40" s="51"/>
-      <c r="Z40" s="51"/>
-      <c r="AA40" s="51"/>
-      <c r="AB40" s="51"/>
-      <c r="AC40" s="51"/>
-      <c r="AD40" s="51"/>
-      <c r="AE40" s="51"/>
-      <c r="AF40" s="51"/>
-      <c r="AG40" s="51"/>
-      <c r="AH40" s="51"/>
-      <c r="AI40" s="51"/>
-      <c r="AJ40" s="51"/>
-      <c r="AK40" s="51"/>
-      <c r="AL40" s="51"/>
-      <c r="AM40" s="51"/>
-      <c r="AN40" s="51"/>
-      <c r="AO40" s="51"/>
-      <c r="AP40" s="51"/>
-      <c r="AQ40" s="51"/>
-      <c r="AR40" s="51"/>
-      <c r="AS40" s="51"/>
-      <c r="AT40" s="51"/>
-      <c r="AU40" s="51"/>
-      <c r="AV40" s="51"/>
-      <c r="AW40" s="51"/>
-      <c r="AX40" s="51"/>
-      <c r="AY40" s="51"/>
-      <c r="AZ40" s="51"/>
-      <c r="BA40" s="51"/>
-      <c r="BB40" s="51"/>
-      <c r="BC40" s="51"/>
-      <c r="BD40" s="51"/>
-      <c r="BE40" s="51"/>
-      <c r="BF40" s="51"/>
-      <c r="BG40" s="51"/>
-      <c r="BH40" s="51"/>
-      <c r="BI40" s="51"/>
-      <c r="BJ40" s="51"/>
-      <c r="BK40" s="51"/>
-      <c r="BL40" s="51"/>
-    </row>
-    <row r="41" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13"/>
-      <c r="B41" s="86"/>
-      <c r="C41" s="87"/>
-      <c r="D41" s="88"/>
-      <c r="E41" s="89"/>
-      <c r="F41" s="89"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="5" t="str">
+      <c r="H40" s="5" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I41" s="45"/>
-      <c r="J41" s="45"/>
-      <c r="K41" s="45"/>
-      <c r="L41" s="45"/>
-      <c r="M41" s="45"/>
-      <c r="N41" s="45"/>
-      <c r="O41" s="45"/>
-      <c r="P41" s="45"/>
-      <c r="Q41" s="45"/>
-      <c r="R41" s="45"/>
-      <c r="S41" s="45"/>
-      <c r="T41" s="45"/>
-      <c r="U41" s="45"/>
-      <c r="V41" s="45"/>
-      <c r="W41" s="45"/>
-      <c r="X41" s="45"/>
-      <c r="Y41" s="45"/>
-      <c r="Z41" s="45"/>
-      <c r="AA41" s="45"/>
-      <c r="AB41" s="45"/>
-      <c r="AC41" s="45"/>
-      <c r="AD41" s="45"/>
-      <c r="AE41" s="45"/>
-      <c r="AF41" s="45"/>
-      <c r="AG41" s="45"/>
-      <c r="AH41" s="45"/>
-      <c r="AI41" s="45"/>
-      <c r="AJ41" s="45"/>
-      <c r="AK41" s="45"/>
-      <c r="AL41" s="45"/>
-      <c r="AM41" s="45"/>
-      <c r="AN41" s="45"/>
-      <c r="AO41" s="45"/>
-      <c r="AP41" s="45"/>
-      <c r="AQ41" s="45"/>
-      <c r="AR41" s="45"/>
-      <c r="AS41" s="45"/>
-      <c r="AT41" s="45"/>
-      <c r="AU41" s="45"/>
-      <c r="AV41" s="45"/>
-      <c r="AW41" s="45"/>
-      <c r="AX41" s="45"/>
-      <c r="AY41" s="45"/>
-      <c r="AZ41" s="45"/>
-      <c r="BA41" s="45"/>
-      <c r="BB41" s="45"/>
-      <c r="BC41" s="45"/>
-      <c r="BD41" s="45"/>
-      <c r="BE41" s="45"/>
-      <c r="BF41" s="45"/>
-      <c r="BG41" s="45"/>
-      <c r="BH41" s="45"/>
-      <c r="BI41" s="45"/>
-      <c r="BJ41" s="45"/>
-      <c r="BK41" s="45"/>
-      <c r="BL41" s="45"/>
-    </row>
-    <row r="42" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="14"/>
-      <c r="B42" s="90" t="s">
+      <c r="I40" s="45"/>
+      <c r="J40" s="45"/>
+      <c r="K40" s="45"/>
+      <c r="L40" s="45"/>
+      <c r="M40" s="45"/>
+      <c r="N40" s="45"/>
+      <c r="O40" s="45"/>
+      <c r="P40" s="45"/>
+      <c r="Q40" s="45"/>
+      <c r="R40" s="45"/>
+      <c r="S40" s="45"/>
+      <c r="T40" s="45"/>
+      <c r="U40" s="45"/>
+      <c r="V40" s="45"/>
+      <c r="W40" s="45"/>
+      <c r="X40" s="45"/>
+      <c r="Y40" s="45"/>
+      <c r="Z40" s="45"/>
+      <c r="AA40" s="45"/>
+      <c r="AB40" s="45"/>
+      <c r="AC40" s="45"/>
+      <c r="AD40" s="45"/>
+      <c r="AE40" s="45"/>
+      <c r="AF40" s="45"/>
+      <c r="AG40" s="45"/>
+      <c r="AH40" s="45"/>
+      <c r="AI40" s="45"/>
+      <c r="AJ40" s="45"/>
+      <c r="AK40" s="45"/>
+      <c r="AL40" s="45"/>
+      <c r="AM40" s="45"/>
+      <c r="AN40" s="45"/>
+      <c r="AO40" s="45"/>
+      <c r="AP40" s="45"/>
+      <c r="AQ40" s="45"/>
+      <c r="AR40" s="45"/>
+      <c r="AS40" s="45"/>
+      <c r="AT40" s="45"/>
+      <c r="AU40" s="45"/>
+      <c r="AV40" s="45"/>
+      <c r="AW40" s="45"/>
+      <c r="AX40" s="45"/>
+      <c r="AY40" s="45"/>
+      <c r="AZ40" s="45"/>
+      <c r="BA40" s="45"/>
+      <c r="BB40" s="45"/>
+      <c r="BC40" s="45"/>
+      <c r="BD40" s="45"/>
+      <c r="BE40" s="45"/>
+      <c r="BF40" s="45"/>
+      <c r="BG40" s="45"/>
+      <c r="BH40" s="45"/>
+      <c r="BI40" s="45"/>
+      <c r="BJ40" s="45"/>
+      <c r="BK40" s="45"/>
+      <c r="BL40" s="45"/>
+    </row>
+    <row r="41" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="14"/>
+      <c r="B41" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="91"/>
-      <c r="D42" s="92"/>
-      <c r="E42" s="93"/>
-      <c r="F42" s="94"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="6" t="str">
+      <c r="C41" s="91"/>
+      <c r="D41" s="92"/>
+      <c r="E41" s="93"/>
+      <c r="F41" s="94"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="6" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I42" s="95"/>
-      <c r="J42" s="95"/>
-      <c r="K42" s="95"/>
-      <c r="L42" s="95"/>
-      <c r="M42" s="95"/>
-      <c r="N42" s="95"/>
-      <c r="O42" s="95"/>
-      <c r="P42" s="95"/>
-      <c r="Q42" s="95"/>
-      <c r="R42" s="95"/>
-      <c r="S42" s="95"/>
-      <c r="T42" s="95"/>
-      <c r="U42" s="95"/>
-      <c r="V42" s="95"/>
-      <c r="W42" s="95"/>
-      <c r="X42" s="95"/>
-      <c r="Y42" s="95"/>
-      <c r="Z42" s="95"/>
-      <c r="AA42" s="95"/>
-      <c r="AB42" s="95"/>
-      <c r="AC42" s="95"/>
-      <c r="AD42" s="95"/>
-      <c r="AE42" s="95"/>
-      <c r="AF42" s="95"/>
-      <c r="AG42" s="95"/>
-      <c r="AH42" s="95"/>
-      <c r="AI42" s="95"/>
-      <c r="AJ42" s="95"/>
-      <c r="AK42" s="95"/>
-      <c r="AL42" s="95"/>
-      <c r="AM42" s="95"/>
-      <c r="AN42" s="95"/>
-      <c r="AO42" s="95"/>
-      <c r="AP42" s="95"/>
-      <c r="AQ42" s="95"/>
-      <c r="AR42" s="95"/>
-      <c r="AS42" s="95"/>
-      <c r="AT42" s="95"/>
-      <c r="AU42" s="95"/>
-      <c r="AV42" s="95"/>
-      <c r="AW42" s="95"/>
-      <c r="AX42" s="95"/>
-      <c r="AY42" s="95"/>
-      <c r="AZ42" s="95"/>
-      <c r="BA42" s="95"/>
-      <c r="BB42" s="95"/>
-      <c r="BC42" s="95"/>
-      <c r="BD42" s="95"/>
-      <c r="BE42" s="95"/>
-      <c r="BF42" s="95"/>
-      <c r="BG42" s="95"/>
-      <c r="BH42" s="95"/>
-      <c r="BI42" s="95"/>
-      <c r="BJ42" s="95"/>
-      <c r="BK42" s="95"/>
-      <c r="BL42" s="95"/>
+      <c r="I41" s="95"/>
+      <c r="J41" s="95"/>
+      <c r="K41" s="95"/>
+      <c r="L41" s="95"/>
+      <c r="M41" s="95"/>
+      <c r="N41" s="95"/>
+      <c r="O41" s="95"/>
+      <c r="P41" s="95"/>
+      <c r="Q41" s="95"/>
+      <c r="R41" s="95"/>
+      <c r="S41" s="95"/>
+      <c r="T41" s="95"/>
+      <c r="U41" s="95"/>
+      <c r="V41" s="95"/>
+      <c r="W41" s="95"/>
+      <c r="X41" s="95"/>
+      <c r="Y41" s="95"/>
+      <c r="Z41" s="95"/>
+      <c r="AA41" s="95"/>
+      <c r="AB41" s="95"/>
+      <c r="AC41" s="95"/>
+      <c r="AD41" s="95"/>
+      <c r="AE41" s="95"/>
+      <c r="AF41" s="95"/>
+      <c r="AG41" s="95"/>
+      <c r="AH41" s="95"/>
+      <c r="AI41" s="95"/>
+      <c r="AJ41" s="95"/>
+      <c r="AK41" s="95"/>
+      <c r="AL41" s="95"/>
+      <c r="AM41" s="95"/>
+      <c r="AN41" s="95"/>
+      <c r="AO41" s="95"/>
+      <c r="AP41" s="95"/>
+      <c r="AQ41" s="95"/>
+      <c r="AR41" s="95"/>
+      <c r="AS41" s="95"/>
+      <c r="AT41" s="95"/>
+      <c r="AU41" s="95"/>
+      <c r="AV41" s="95"/>
+      <c r="AW41" s="95"/>
+      <c r="AX41" s="95"/>
+      <c r="AY41" s="95"/>
+      <c r="AZ41" s="95"/>
+      <c r="BA41" s="95"/>
+      <c r="BB41" s="95"/>
+      <c r="BC41" s="95"/>
+      <c r="BD41" s="95"/>
+      <c r="BE41" s="95"/>
+      <c r="BF41" s="95"/>
+      <c r="BG41" s="95"/>
+      <c r="BH41" s="95"/>
+      <c r="BI41" s="95"/>
+      <c r="BJ41" s="95"/>
+      <c r="BK41" s="95"/>
+      <c r="BL41" s="95"/>
+    </row>
+    <row r="42" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G43" s="3"/>
+      <c r="C43" s="16"/>
+      <c r="F43" s="15"/>
     </row>
     <row r="44" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="16"/>
-      <c r="F44" s="15"/>
-    </row>
-    <row r="45" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C45" s="4"/>
+      <c r="C44" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
     <mergeCell ref="BF7:BL7"/>
     <mergeCell ref="I7:O7"/>
     <mergeCell ref="P7:V7"/>
@@ -4988,18 +4951,8 @@
     <mergeCell ref="AK7:AQ7"/>
     <mergeCell ref="AR7:AX7"/>
     <mergeCell ref="AY7:BE7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
   </mergeCells>
-  <conditionalFormatting sqref="D10:D42">
+  <conditionalFormatting sqref="D10:D41">
     <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5013,7 +4966,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL40">
+  <conditionalFormatting sqref="I7:BL39">
     <cfRule type="expression" dxfId="8" priority="1">
       <formula>AND(TODAY()&gt;=I$8, TODAY()&lt;J$8)</formula>
     </cfRule>
@@ -5026,7 +4979,7 @@
       <formula>AND(task_end&gt;=I$8,task_start&lt;J$8)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18:BL22 I24:BL28">
+  <conditionalFormatting sqref="I18:BL21 I23:BL27">
     <cfRule type="expression" dxfId="5" priority="4">
       <formula>AND(task_start&lt;=I$8,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$8)</formula>
     </cfRule>
@@ -5034,7 +4987,7 @@
       <formula>AND(task_end&gt;=I$8,task_start&lt;J$8)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I30:BL34">
+  <conditionalFormatting sqref="I29:BL33">
     <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND(task_start&lt;=I$8,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$8)</formula>
     </cfRule>
@@ -5042,7 +4995,7 @@
       <formula>AND(task_end&gt;=I$8,task_start&lt;J$8)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36:BL40">
+  <conditionalFormatting sqref="I35:BL39">
     <cfRule type="expression" dxfId="1" priority="36">
       <formula>AND(task_start&lt;=I$8,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$8)</formula>
     </cfRule>
@@ -5062,10 +5015,10 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B8 contains the Phase 1 sample title. Enter a new title in cell B8._x000a_To delete the phase and work only from tasks, simply delete this row." sqref="A11" xr:uid="{CEC78982-AFA8-419E-B0A2-676B709E5100}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="B9 contains the task name.  C9 is the assignee.  D9 is a progress bar that shades based on the number entered into the cell.  _x000a__x000a_E9 contains the start date and F9 contains the end date._x000a__x000a_The Gantt chart will fill in starting in cell I9 based on task dates." sqref="A12" xr:uid="{D870A2F6-6B07-4F5A-A81D-4BCCFADF8796}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Rows 10 through 13 repeat the pattern from row 9. _x000a__x000a_Repeat the instructions from cell A9 for all task rows in this worksheet. _x000a__x000a_Continue entering tasks in cells A10 through A13 or go to cell A14 to learn more." sqref="A13" xr:uid="{872449A7-C3CC-45B6-BA90-B1AAD66BA0E5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B14 contains the Phase 2 sample title. Enter a new title in cell B14._x000a_To delete the phase and work only from tasks, simply delete this row. To remove the phase, simply delete the row. Add tasks to previous phase by entering a new row above this one._x000a_" sqref="A17 A23" xr:uid="{4F48FC41-E335-47F1-87AA-3333A52AD81C}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A29" xr:uid="{956902D1-D3B5-416D-BB69-9362D193BC0A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A35" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A42" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B14 contains the Phase 2 sample title. Enter a new title in cell B14._x000a_To delete the phase and work only from tasks, simply delete this row. To remove the phase, simply delete the row. Add tasks to previous phase by entering a new row above this one._x000a_" sqref="A17 A22" xr:uid="{4F48FC41-E335-47F1-87AA-3333A52AD81C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A28" xr:uid="{956902D1-D3B5-416D-BB69-9362D193BC0A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A34" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A41" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
@@ -5074,7 +5027,7 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="F21 F31:F32 E32 F37" formula="1"/>
+    <ignoredError sqref="F36" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -5092,7 +5045,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D10:D42</xm:sqref>
+          <xm:sqref>D10:D41</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -5225,35 +5178,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5565,34 +5489,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A09426A3-87E9-4865-8A6C-3456B026AE03}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5613,6 +5539,33 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>